<commit_message>
Add latches to diagnostics output
</commit_message>
<xml_diff>
--- a/DiagnosticsInputs.xlsx
+++ b/DiagnosticsInputs.xlsx
@@ -252,11 +252,11 @@
   </sheetPr>
   <dimension ref="A1:I1461"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C136" activeCellId="0" sqref="C136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="18.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2218,7 +2218,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G68" s="3" t="n">
         <v>0</v>
@@ -2595,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G81" s="3" t="n">
         <v>0</v>
@@ -2624,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G82" s="3" t="n">
         <v>0</v>
@@ -4152,7 +4152,7 @@
         <v>100</v>
       </c>
       <c r="C135" s="3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D135" s="3" t="n">
         <v>0</v>

</xml_diff>